<commit_message>
Update to Godot 4.2
</commit_message>
<xml_diff>
--- a/godot-luban-data/Configs/_示例.xlsx
+++ b/godot-luban-data/Configs/_示例.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23220" windowHeight="11915"/>
+    <workbookView windowWidth="23676" windowHeight="11195"/>
   </bookViews>
   <sheets>
     <sheet name="基础" sheetId="1" r:id="rId1"/>
@@ -304,7 +304,7 @@
     <t>some_double_value</t>
   </si>
   <si>
-    <t>some_vec3</t>
+    <t>#some_vec3</t>
   </si>
   <si>
     <t>##type</t>
@@ -472,7 +472,7 @@
     <t>some_array_3</t>
   </si>
   <si>
-    <t>some_array_4</t>
+    <t>#some_array_4</t>
   </si>
   <si>
     <t>some_map_1</t>
@@ -616,14 +616,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -640,6 +640,19 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.5"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.5"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
     </font>
@@ -1134,137 +1147,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1273,23 +1286,30 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1606,7 +1626,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1623,47 +1643,47 @@
     <col min="10" max="10" width="20.8888888888889" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
     <col min="12" max="12" width="20.5555555555556" customWidth="1"/>
-    <col min="13" max="13" width="17.6666666666667" customWidth="1"/>
+    <col min="13" max="13" width="17.6666666666667" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.6" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1671,40 +1691,40 @@
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1712,69 +1732,69 @@
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" ht="15.6" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" ht="15.6" spans="1:13">
       <c r="A5" s="3"/>
-      <c r="B5" s="5">
+      <c r="B5" s="8">
         <v>1001</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1798,7 +1818,7 @@
       <c r="I5" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="10" t="s">
         <v>42</v>
       </c>
       <c r="K5" s="3">
@@ -1807,22 +1827,22 @@
       <c r="L5" s="3">
         <v>42.332</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" ht="15.6" spans="1:13">
       <c r="A6" s="3"/>
-      <c r="B6" s="5">
+      <c r="B6" s="8">
         <v>2001</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="8">
         <v>1</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="8">
         <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -1831,13 +1851,13 @@
       <c r="G6" s="3">
         <v>112.5</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="5" t="b">
+      <c r="I6" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="10" t="s">
         <v>47</v>
       </c>
       <c r="K6" s="3">
@@ -1846,22 +1866,22 @@
       <c r="L6" s="3">
         <v>12.332</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="7" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" ht="15.6" spans="1:13">
       <c r="A7" s="3"/>
-      <c r="B7" s="5">
+      <c r="B7" s="8">
         <v>3001</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="8">
         <v>2</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="8">
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -1870,13 +1890,13 @@
       <c r="G7" s="3">
         <v>50</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="5" t="b">
+      <c r="I7" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="10" t="s">
         <v>52</v>
       </c>
       <c r="K7" s="3">
@@ -1885,252 +1905,252 @@
       <c r="L7" s="3">
         <v>1238.897543</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" ht="15.6" spans="1:13">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="10">
         <v>3002</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" ht="15.6" spans="1:13">
       <c r="A9" s="3"/>
-      <c r="B9" s="5">
+      <c r="B9" s="8">
         <v>3003</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="8">
         <v>1</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="8">
         <v>1</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="8" t="s">
         <v>56</v>
       </c>
       <c r="G9" s="3">
         <v>10</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="5" t="b">
+      <c r="I9" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="10" t="s">
         <v>57</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="3" t="s">
+      <c r="M9" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" ht="15.6" spans="1:13">
       <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="7"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="10"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
+      <c r="M10" s="7"/>
     </row>
     <row r="11" ht="15.6" spans="1:13">
       <c r="A11" s="3"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="7"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="10"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
+      <c r="M11" s="7"/>
     </row>
     <row r="12" ht="15.6" spans="1:13">
       <c r="A12" s="3"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="7"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="10"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="M12" s="7"/>
     </row>
     <row r="13" ht="15.6" spans="1:13">
       <c r="A13" s="3"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="7"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="10"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
+      <c r="M13" s="7"/>
     </row>
     <row r="14" ht="15.6" spans="1:13">
       <c r="A14" s="3"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="7"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="10"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="M14" s="7"/>
     </row>
     <row r="15" ht="15.6" spans="1:13">
       <c r="A15" s="3"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="7"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="10"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="M15" s="7"/>
     </row>
     <row r="16" ht="15.6" spans="1:13">
       <c r="A16" s="3"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="7"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="10"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+      <c r="M16" s="7"/>
     </row>
     <row r="17" ht="15.6" spans="1:13">
       <c r="A17" s="3"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="7"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="10"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
+      <c r="M17" s="7"/>
     </row>
     <row r="18" ht="15.6" spans="1:13">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="7"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="10"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
+      <c r="M18" s="7"/>
     </row>
     <row r="19" ht="15.6" spans="1:13">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="8" t="s">
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="11" t="s">
         <v>61</v>
       </c>
       <c r="G19" s="3"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="7"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="10"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+      <c r="M19" s="7"/>
     </row>
     <row r="20" ht="15.6" spans="1:13">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="7"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="10"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="M20" s="7"/>
     </row>
     <row r="22" ht="15.6" spans="1:2">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="8" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2151,8 +2171,8 @@
   <sheetPr/>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5"/>
@@ -2160,7 +2180,7 @@
     <col min="2" max="2" width="28.7777777777778" customWidth="1"/>
     <col min="3" max="3" width="32.5555555555556" customWidth="1"/>
     <col min="4" max="4" width="34.4444444444444" customWidth="1"/>
-    <col min="5" max="5" width="32.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="32.6666666666667" style="4" customWidth="1"/>
     <col min="6" max="6" width="38.7777777777778" customWidth="1"/>
     <col min="7" max="7" width="9.22222222222222" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
@@ -2173,30 +2193,30 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2204,30 +2224,30 @@
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2235,34 +2255,34 @@
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="5" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2277,7 +2297,7 @@
       <c r="D4" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -2310,7 +2330,7 @@
       <c r="D5" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="7" t="s">
         <v>102</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -2337,7 +2357,7 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>

</xml_diff>